<commit_message>
Update Bill of Materials Penduino Daugterboard.xlsx
</commit_message>
<xml_diff>
--- a/pendulum_daughterboard/Bill of Materials Penduino Daugterboard.xlsx
+++ b/pendulum_daughterboard/Bill of Materials Penduino Daugterboard.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
   <si>
     <t>Component Name</t>
   </si>
@@ -47,33 +47,12 @@
     <t>IC5</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>D4</t>
   </si>
   <si>
     <t>J4</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -104,12 +83,6 @@
     <t>SW1</t>
   </si>
   <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
@@ -138,13 +111,151 @@
   </si>
   <si>
     <t>Q2</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Requisition Number</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Logic IC NAND Gate</t>
+  </si>
+  <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>MC74ACT00DG</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/on-semiconductor/mc74act00dg/ic-quad-nand-gate-2i-p-soic-14/dp/1652018?st=2%20input%20nand%20gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>logic IC AND Gate</t>
+  </si>
+  <si>
+    <t>MC74HC32ADG</t>
+  </si>
+  <si>
+    <t>Logic IC OR Gate</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/on-semiconductor/mc74hc32adg/ic-74hc-cmos-smd-74hc32-soic14/dp/9666966?st=2%20input%20or%20gate</t>
+  </si>
+  <si>
+    <t>MC74HC08ADG</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/on-semiconductor/mc74hc08adg/ic-74hc-cmos-smd-74hc08-soic14/dp/9666907</t>
+  </si>
+  <si>
+    <t>RS Components</t>
+  </si>
+  <si>
+    <t>ATTINY85-20SF</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/microcontrollers/1717852/?relevancy-data=7365617263685F636173636164655F6F726465723D31267365617263685F696E746572666163655F6E616D653D4931384E525353746F636B4E756D626572267365617263685F6C616E67756167655F757365643D656E26736561726</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>MP008291</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>LED Green</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/multicomp-pro/mp008291/led-green-70mcd-576nm-0805/dp/3796323?st=0805%20smd%20led</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/maxim-integrated-products/max9928faua/current-sense-amp-0-1-28v-8umax/dp/2519050?st=max9928</t>
+  </si>
+  <si>
+    <t>MAX9928FAUA+</t>
+  </si>
+  <si>
+    <t>Current Sense Amplifier</t>
+  </si>
+  <si>
+    <t>D1,D2, D3</t>
+  </si>
+  <si>
+    <t>Unit Price (ex. VAT)</t>
+  </si>
+  <si>
+    <t>R1, R2, R3</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>120 OHM resistor for the LED circuit</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/panasonic/era6aeb121v/res-120r-0-125w-0805-metal-film/dp/1577646?st=0805%20resistor</t>
+  </si>
+  <si>
+    <t>ERA6AEB121V</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>2k2</t>
+  </si>
+  <si>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>1614917-1</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/neohm-te-connectivity/1614917-1/res-2k2-0-1-0-1w-0805-thin-film/dp/2992213?st=7.R</t>
+  </si>
+  <si>
+    <t>RS73F2ATTD1003B</t>
+  </si>
+  <si>
+    <t>https://uk.farnell.com/koa-speer-electronics/rs73f2attd1003b/res-100k-0-1-0-25w-thick-film/dp/3947030?st=0805%20resistor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,13 +263,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -170,13 +301,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,20 +591,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,202 +618,538 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2">
+        <v>0.63</v>
+      </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
       <c r="B4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4">
+        <v>0.68</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5">
+        <v>0.68</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6">
+        <v>1.88</v>
+      </c>
+      <c r="K6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
       <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7">
+        <v>132</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7">
+        <v>0.11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <v>132</v>
+      </c>
+      <c r="D9">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9">
+        <v>0.27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10">
+        <v>0.17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11">
+        <v>0.18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>44</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="K26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="D28" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" t="s">
-        <v>32</v>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28">
+        <v>1.8140000000000001</v>
+      </c>
+      <c r="K28" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1"/>
+    <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="H2" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="H28" r:id="rId5"/>
+    <hyperlink ref="H7" r:id="rId6"/>
+    <hyperlink ref="H6" r:id="rId7"/>
+    <hyperlink ref="H9" r:id="rId8"/>
+    <hyperlink ref="H10" r:id="rId9"/>
+    <hyperlink ref="H11" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>